<commit_message>
agregue discreta y sus correlativas :D
</commit_message>
<xml_diff>
--- a/Materias/Materias.xlsx
+++ b/Materias/Materias.xlsx
@@ -234,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,12 +259,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -278,13 +272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -616,7 +609,7 @@
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -801,7 +794,7 @@
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -846,7 +839,7 @@
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>